<commit_message>
Add outputs given new probabilities for public perception
</commit_message>
<xml_diff>
--- a/dtree/outputs/mag_proba_sensitivity.xlsx
+++ b/dtree/outputs/mag_proba_sensitivity.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>747.0882562132138</v>
+        <v>701.3070661196912</v>
       </c>
     </row>
     <row r="3">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>747.0882562132138</v>
+        <v>701.3070661196912</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>791.2827089433745</v>
+        <v>743.3819643578375</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>881.1640147916739</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>973.1114995737557</v>
+        <v>916.252090899261</v>
       </c>
     </row>
     <row r="7">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1067.222396931845</v>
+        <v>1005.571982782548</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1163.600969911488</v>
+        <v>1096.932028729645</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1262.359205305958</v>
+        <v>1190.427609826836</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1363.617595907754</v>
+        <v>1286.160956459582</v>
       </c>
     </row>
     <row r="11">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1467.506024370215</v>
+        <v>1384.241820224659</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="14">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="15">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="16">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>973.1114995737557</v>
+        <v>916.252090899261</v>
       </c>
     </row>
     <row r="17">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1067.222396931845</v>
+        <v>1005.571982782548</v>
       </c>
     </row>
     <row r="18">
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1163.600969911488</v>
+        <v>1096.932028729645</v>
       </c>
     </row>
     <row r="19">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1262.359205305958</v>
+        <v>1190.427609826836</v>
       </c>
     </row>
     <row r="20">
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1363.617595907754</v>
+        <v>1286.160956459582</v>
       </c>
     </row>
     <row r="21">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1467.506024370215</v>
+        <v>1384.241820224659</v>
       </c>
     </row>
     <row r="22">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="24">
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="25">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>881.1640147916751</v>
+        <v>828.8832227764427</v>
       </c>
     </row>
     <row r="26">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>973.1114995737557</v>
+        <v>916.252090899261</v>
       </c>
     </row>
     <row r="27">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1067.222396931845</v>
+        <v>1005.571982782548</v>
       </c>
     </row>
     <row r="28">
@@ -938,7 +938,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1163.600969911488</v>
+        <v>1096.932028729645</v>
       </c>
     </row>
     <row r="29">
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1262.359205305958</v>
+        <v>1190.427609826836</v>
       </c>
     </row>
     <row r="30">
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1363.617595907754</v>
+        <v>1286.160956459582</v>
       </c>
     </row>
     <row r="31">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1467.506024370215</v>
+        <v>1384.241820224659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update probabilities and all resulting files
</commit_message>
<xml_diff>
--- a/dtree/outputs/mag_proba_sensitivity.xlsx
+++ b/dtree/outputs/mag_proba_sensitivity.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>701.3070661196912</v>
+        <v>937.5377473015355</v>
       </c>
     </row>
     <row r="3">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>701.3070661196912</v>
+        <v>937.5377473015355</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>743.3819643578375</v>
+        <v>996.2938725423382</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>916.252090899261</v>
+        <v>1240.349233061726</v>
       </c>
     </row>
     <row r="7">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1005.571982782548</v>
+        <v>1368.198052860202</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1096.932028729645</v>
+        <v>1500.268506819392</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1190.427609826836</v>
+        <v>1636.848944567762</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1286.160956459582</v>
+        <v>1778.258306167385</v>
       </c>
     </row>
     <row r="11">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1384.241820224659</v>
+        <v>1924.850608277711</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="14">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="15">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="16">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>916.252090899261</v>
+        <v>1240.349233061726</v>
       </c>
     </row>
     <row r="17">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1005.571982782548</v>
+        <v>1368.198052860202</v>
       </c>
     </row>
     <row r="18">
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1096.932028729645</v>
+        <v>1500.268506819392</v>
       </c>
     </row>
     <row r="19">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1190.427609826836</v>
+        <v>1636.848944567762</v>
       </c>
     </row>
     <row r="20">
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1286.160956459582</v>
+        <v>1778.258306167385</v>
       </c>
     </row>
     <row r="21">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1384.241820224659</v>
+        <v>1924.850608277711</v>
       </c>
     </row>
     <row r="22">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="24">
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="25">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>828.8832227764427</v>
+        <v>1116.460497103601</v>
       </c>
     </row>
     <row r="26">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>916.252090899261</v>
+        <v>1240.349233061726</v>
       </c>
     </row>
     <row r="27">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1005.571982782548</v>
+        <v>1368.198052860202</v>
       </c>
     </row>
     <row r="28">
@@ -938,7 +938,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1096.932028729645</v>
+        <v>1500.268506819392</v>
       </c>
     </row>
     <row r="29">
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1190.427609826836</v>
+        <v>1636.848944567762</v>
       </c>
     </row>
     <row r="30">
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1286.160956459582</v>
+        <v>1778.258306167385</v>
       </c>
     </row>
     <row r="31">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1384.241820224659</v>
+        <v>1924.850608277711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>